<commit_message>
Changed graph to be bar graph
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -177,8 +177,9 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -195,29 +196,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:trendline>
             <c:spPr>
               <a:ln w="19050" cap="rnd">
@@ -232,7 +219,7 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
-          <c:xVal>
+          <c:cat>
             <c:numRef>
               <c:f>Sheet1!$A$4:$A$9</c:f>
               <c:numCache>
@@ -258,8 +245,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
+          </c:cat>
+          <c:val>
             <c:numRef>
               <c:f>Sheet1!$B$4:$B$9</c:f>
               <c:numCache>
@@ -285,8 +272,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
+          </c:val>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -303,29 +289,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:trendline>
             <c:spPr>
               <a:ln w="19050" cap="rnd">
@@ -340,7 +312,7 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
-          <c:xVal>
+          <c:cat>
             <c:numRef>
               <c:f>Sheet1!$A$4:$A$9</c:f>
               <c:numCache>
@@ -366,8 +338,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
+          </c:cat>
+          <c:val>
             <c:numRef>
               <c:f>Sheet1!$C$4:$C$9</c:f>
               <c:numCache>
@@ -393,8 +365,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
+          </c:val>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -404,11 +375,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2123067824"/>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2096209856"/>
         <c:axId val="-2123062464"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="-2123067824"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2096209856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -527,8 +499,11 @@
         </c:txPr>
         <c:crossAx val="-2123062464"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="-2123062464"/>
         <c:scaling>
@@ -648,9 +623,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2123067824"/>
+        <c:crossAx val="-2096209856"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>

</xml_diff>